<commit_message>
Cleaned up dataframe to be analysed
removed rows with missing value in prefLabel
Convert prefLabel to string
</commit_message>
<xml_diff>
--- a/examples/ontology-from-excel/tool/onto.xlsx
+++ b/examples/ontology-from-excel/tool/onto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sintef.sharepoint.com/teams/work-15746/Shared Documents/emmontopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{65CBBF81-7317-4A2C-B962-E0FE5505277D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB4979CB-F2A8-4BCA-8453-F401C92DD583}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{65CBBF81-7317-4A2C-B962-E0FE5505277D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5D64487-F050-4DA9-8DFA-208299A2AC03}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{2EA941AB-E9B1-4DC5-9547-722248AB830E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
   <si>
     <t>Concept</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>hasPart some TemporalBoundary;hasProperty some Time</t>
+  </si>
+  <si>
+    <t>Number</t>
   </si>
 </sst>
 </file>
@@ -862,10 +865,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D645D5-E8F4-4C20-A45A-A7B2168B3691}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,19 +1127,27 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1150,12 +1161,67 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <CorpSiteZipContact xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectLeader xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectLeader>
+    <CorpSiteSubTitle xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteTags xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteISBN xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowFeedback xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteAccess xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Kun navngitte medlemmer</CorpSiteAccess>
+    <CorpSiteRecipientPerson xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectName xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocInstitute xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteInstitutePhone xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectOwner xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectOwner>
+    <CorpDocPageClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocPageClassificationNbNo>
+    <CorpDocClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocClassificationEnUs>
+    <CorpDocClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocClassificationNbNo>
+    <CorpSiteClassification xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpSiteClassification>
+    <CorpSiteInstituteEmail xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteCoAuthors xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteDocumentAuthor xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteDocumentAuthor>
+    <CorpSiteInstituteEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteRecipientCompany xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteDocLanguage xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocVersion xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowApproval xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <ArchiveStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectQA xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectQA>
+    <CorpSiteZipAddress xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteVATNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteReportNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteOurRef xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocPageClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocPageClassificationEnUs>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1678,73 +1744,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <CorpSiteZipContact xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectLeader xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectLeader>
-    <CorpSiteSubTitle xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteTags xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteISBN xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowFeedback xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteAccess xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Kun navngitte medlemmer</CorpSiteAccess>
-    <CorpSiteRecipientPerson xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectName xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocInstitute xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteInstitutePhone xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectOwner xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectOwner>
-    <CorpDocPageClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocPageClassificationNbNo>
-    <CorpDocClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocClassificationEnUs>
-    <CorpDocClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocClassificationNbNo>
-    <CorpSiteClassification xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpSiteClassification>
-    <CorpSiteInstituteEmail xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteCoAuthors xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteDocumentAuthor xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteDocumentAuthor>
-    <CorpSiteInstituteEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteRecipientCompany xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteDocLanguage xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocVersion xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowApproval xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <ArchiveStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectQA xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectQA>
-    <CorpSiteZipAddress xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteVATNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteReportNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteOurRef xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocPageClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocPageClassificationEnUs>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5504F3-8457-4CD0-9BA4-F4E5EEC4ABF3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95E916DF-5697-4D04-9AE8-BCDE5705DE19}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="f0e54009-8c9c-44b5-8b9b-dd795f6c992f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8bbd4995-53b7-43e2-b62f-10947586ac31"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c4cb6b28-ce9b-4437-9d9c-1e653dd193be"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1770,19 +1791,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95E916DF-5697-4D04-9AE8-BCDE5705DE19}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5504F3-8457-4CD0-9BA4-F4E5EEC4ABF3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f0e54009-8c9c-44b5-8b9b-dd795f6c992f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8bbd4995-53b7-43e2-b62f-10947586ac31"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="c4cb6b28-ce9b-4437-9d9c-1e653dd193be"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added import ontologies from excel
</commit_message>
<xml_diff>
--- a/examples/ontology-from-excel/tool/onto.xlsx
+++ b/examples/ontology-from-excel/tool/onto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sintef.sharepoint.com/teams/work-15746/Shared Documents/emmontopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{65CBBF81-7317-4A2C-B962-E0FE5505277D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5D64487-F050-4DA9-8DFA-208299A2AC03}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{65CBBF81-7317-4A2C-B962-E0FE5505277D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D95410AF-0C55-4E68-B3D7-8422E140B86B}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{2EA941AB-E9B1-4DC5-9547-722248AB830E}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{2EA941AB-E9B1-4DC5-9547-722248AB830E}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="82">
   <si>
     <t>Concept</t>
   </si>
@@ -272,6 +272,15 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>http://emmo.info/emmo/domain/onto</t>
+  </si>
+  <si>
+    <t>http://emmo.info/emmo/domain/onto/0.01</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/emmo-repo/emmo-repo.github.io/master/versions/1.0.0-beta/emmo-inferred-chemistry2.ttl</t>
   </si>
 </sst>
 </file>
@@ -724,14 +733,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEECC088-989A-4277-A366-69DAA3CBC81F}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="102.7109375" customWidth="1"/>
+    <col min="2" max="2" width="120.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -750,19 +759,27 @@
       <c r="A2" s="12" t="s">
         <v>25</v>
       </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
       <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="B4">
+        <v>0.01</v>
+      </c>
       <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -828,6 +845,9 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>81</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>40</v>
@@ -867,7 +887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D645D5-E8F4-4C20-A45A-A7B2168B3691}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1161,67 +1181,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <CorpSiteZipContact xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectLeader xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectLeader>
-    <CorpSiteSubTitle xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteTags xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteISBN xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowFeedback xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteAccess xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Kun navngitte medlemmer</CorpSiteAccess>
-    <CorpSiteRecipientPerson xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectName xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocInstitute xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteInstitutePhone xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectOwner xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectOwner>
-    <CorpDocPageClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocPageClassificationNbNo>
-    <CorpDocClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocClassificationEnUs>
-    <CorpDocClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocClassificationNbNo>
-    <CorpSiteClassification xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpSiteClassification>
-    <CorpSiteInstituteEmail xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteCoAuthors xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteDocumentAuthor xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteDocumentAuthor>
-    <CorpSiteInstituteEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteRecipientCompany xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteDocLanguage xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocVersion xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowApproval xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <ArchiveStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectQA xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectQA>
-    <CorpSiteZipAddress xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteVATNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteReportNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteOurRef xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocPageClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocPageClassificationEnUs>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1744,28 +1709,73 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <CorpSiteZipContact xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectLeader xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectLeader>
+    <CorpSiteSubTitle xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteTags xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteISBN xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowFeedback xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteAccess xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Kun navngitte medlemmer</CorpSiteAccess>
+    <CorpSiteRecipientPerson xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectName xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocInstitute xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteInstitutePhone xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectOwner xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectOwner>
+    <CorpDocPageClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocPageClassificationNbNo>
+    <CorpDocClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocClassificationEnUs>
+    <CorpDocClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocClassificationNbNo>
+    <CorpSiteClassification xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpSiteClassification>
+    <CorpSiteInstituteEmail xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteCoAuthors xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteDocumentAuthor xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteDocumentAuthor>
+    <CorpSiteInstituteEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteRecipientCompany xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteDocLanguage xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocVersion xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowApproval xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <ArchiveStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectQA xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectQA>
+    <CorpSiteZipAddress xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteVATNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteReportNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteOurRef xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocPageClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocPageClassificationEnUs>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95E916DF-5697-4D04-9AE8-BCDE5705DE19}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5504F3-8457-4CD0-9BA4-F4E5EEC4ABF3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f0e54009-8c9c-44b5-8b9b-dd795f6c992f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8bbd4995-53b7-43e2-b62f-10947586ac31"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="c4cb6b28-ce9b-4437-9d9c-1e653dd193be"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1791,9 +1801,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5504F3-8457-4CD0-9BA4-F4E5EEC4ABF3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95E916DF-5697-4D04-9AE8-BCDE5705DE19}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="f0e54009-8c9c-44b5-8b9b-dd795f6c992f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8bbd4995-53b7-43e2-b62f-10947586ac31"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c4cb6b28-ce9b-4437-9d9c-1e653dd193be"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>